<commit_message>
started on a new model :)))) agony
</commit_message>
<xml_diff>
--- a/thruster_data.xlsx
+++ b/thruster_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\szeke\Documents\DARE\arc_optimization\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{734D9074-F729-4A8C-9328-27613AD846BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A7671F8-7231-41E3-AE55-4A6E34C64F3F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="13900" xr2:uid="{14AF24CB-EEC9-4C32-8C0C-4528929FB34A}"/>
   </bookViews>
@@ -472,7 +472,7 @@
   <dimension ref="A1:I16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M15" sqref="M15"/>
+      <selection activeCell="L15" sqref="L15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>